<commit_message>
added gecko driver; added string split to capture 7th page in results
</commit_message>
<xml_diff>
--- a/CTDC_Automation/TestData/Input_TestData.xlsx
+++ b/CTDC_Automation/TestData/Input_TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\DataCommons_Automation\CTDC_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B2D902-EF5E-4B6A-B8A0-C02789D3D12C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F59613-F202-471C-9262-2F733933EFA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>Environment</t>
   </si>
@@ -112,9 +112,6 @@
     <t>https://trialcommons-qa.cancer.gov/#/</t>
   </si>
   <si>
-    <t>C:\Users\lollal\Testcomplete\DataForTestCase\ICDC_data\Trial_Test1Data.xlsx</t>
-  </si>
-  <si>
     <t>InitialLoad</t>
   </si>
   <si>
@@ -155,6 +152,12 @@
   </si>
   <si>
     <t>https://caninecommons.cancer.gov/#/</t>
+  </si>
+  <si>
+    <t>C:\Users\radhakrishnang2\Desktop\DataCommons_Automation\CTDC_Automation\TestData\DatafromNeo4j.xlsx</t>
+  </si>
+  <si>
+    <t>Firefox</t>
   </si>
 </sst>
 </file>
@@ -530,20 +533,20 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="70.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
+    <col min="4" max="4" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="98" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -566,7 +569,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -586,7 +589,7 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -603,19 +606,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C468257-9521-42A0-A4DB-E0691FA7FE45}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" customWidth="1"/>
-    <col min="7" max="7" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.7265625" customWidth="1"/>
+    <col min="7" max="7" width="54.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -632,10 +635,10 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
         <v>28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -650,17 +653,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="J2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -669,33 +672,33 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" t="s">
         <v>32</v>
-      </c>
-      <c r="J3" t="s">
-        <v>33</v>
       </c>
       <c r="K3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -707,30 +710,30 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
         <v>30</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
         <v>31</v>
       </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>32</v>
-      </c>
-      <c r="J4" t="s">
-        <v>33</v>
       </c>
       <c r="K4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -739,33 +742,33 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" t="s">
         <v>32</v>
-      </c>
-      <c r="J5" t="s">
-        <v>33</v>
       </c>
       <c r="K5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -774,22 +777,22 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
         <v>38</v>
       </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s">
-        <v>39</v>
-      </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K6" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
updates: adding page 7 in ui results table; arraylists comparison added
</commit_message>
<xml_diff>
--- a/CTDC_Automation/TestData/Input_TestData.xlsx
+++ b/CTDC_Automation/TestData/Input_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\DataCommons_Automation\CTDC_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F59613-F202-471C-9262-2F733933EFA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA8C602-72F6-466B-8643-D08130D83B88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -533,7 +533,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C468257-9521-42A0-A4DB-E0691FA7FE45}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>